<commit_message>
feature branches for transaction
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/sample/So_quy_tien_mat.xlsx
+++ b/src/main/resources/templates/sample/So_quy_tien_mat.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SongLamEdu\src\main\resources\templates\sample\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250CEE73-F381-490F-9A0F-5813ACB037FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SỔ QUỸ TIỀN MẶT" sheetId="1" r:id="rId2"/>
+    <sheet name="SỔ QUỸ TIỀN MẶT" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>Ngày, tháng ghi sổ</t>
   </si>
@@ -90,27 +95,26 @@
   </si>
   <si>
     <t>Tổng cộng</t>
+  </si>
+  <si>
+    <t>Cơ sở</t>
+  </si>
+  <si>
+    <t>Cơ sở 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="177" formatCode="#,##0_);(#,##0)"/>
-    <numFmt numFmtId="178" formatCode="dd/MM/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0_);\(#,##0\)"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -190,6 +194,7 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -202,6 +207,7 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -214,6 +220,7 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -226,6 +233,7 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -238,6 +246,7 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -248,252 +257,118 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+  <cellXfs count="28">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -793,302 +668,321 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{de0ad852-fc06-465a-99af-2b79ccc49185}">
-  <dimension ref="A1:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0AD852-FC06-465A-99AF-2B79CCC49185}">
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.428571428571427" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.857142857142858" style="1" customWidth="1"/>
-    <col min="3" max="4" width="17" style="2" customWidth="1"/>
-    <col min="5" max="5" width="35.57142857142857" style="2" customWidth="1"/>
-    <col min="6" max="8" width="17" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17" style="2" customWidth="1"/>
-    <col min="10" max="10" width="28.428571428571427" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="8" customWidth="1"/>
+    <col min="3" max="4" width="17" style="9" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" style="9" customWidth="1"/>
+    <col min="6" max="8" width="17" style="10" customWidth="1"/>
+    <col min="9" max="9" width="17" style="9" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="13" customFormat="1" ht="28.25" customHeight="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:11" s="12" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-    </row>
-    <row r="2" spans="1:10" s="17" customFormat="1" ht="28.25" customHeight="1">
-      <c r="A2" s="14" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" s="13" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="1:10" s="13" customFormat="1" ht="15">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" ht="15">
-      <c r="A4" s="5" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" s="12" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="5" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15">
+      <c r="K4" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="33" t="s">
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="34">
+      <c r="F6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="19">
         <v>0</v>
       </c>
-      <c r="I6" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15">
-      <c r="A7" s="35">
+      <c r="I6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
         <v>45992</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="20">
         <v>45992</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="36" t="s">
+      <c r="D7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="22">
         <v>350000</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="22">
         <v>0</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="22">
         <v>350000</v>
       </c>
-      <c r="I7" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="36" t="s">
+      <c r="I7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15">
-      <c r="A8" s="35">
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
         <v>45998</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="20">
         <v>45998</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="36" t="s">
+      <c r="D8" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="22">
         <v>350000</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="22">
         <v>0</v>
       </c>
-      <c r="H8" s="37">
+      <c r="H8" s="22">
         <v>700000</v>
       </c>
-      <c r="I8" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="36" t="s">
+      <c r="I8" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15">
-      <c r="A9" s="35">
+      <c r="K8" s="26"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
         <v>45998</v>
       </c>
-      <c r="B9" s="35">
+      <c r="B9" s="20">
         <v>45998</v>
       </c>
-      <c r="C9" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="36" t="s">
+      <c r="C9" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="22">
         <v>0</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="22">
         <v>1000000</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="23">
         <v>-300000</v>
       </c>
-      <c r="I9" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="36" t="s">
+      <c r="I9" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15">
-      <c r="A10" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="40" t="s">
+      <c r="K9" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="41">
+      <c r="F10" s="19">
         <v>700000</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G10" s="19">
         <v>1000000</v>
       </c>
-      <c r="H10" s="42">
+      <c r="H10" s="24">
         <v>-300000</v>
       </c>
-      <c r="I10" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15">
-      <c r="A11" s="27" t="s">
+      <c r="I10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="25"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="31">
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16">
         <v>700000</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="16">
         <v>1000000</v>
       </c>
-      <c r="H11" s="31"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.39370078740157477" right="0.39370078740157477" top="0.39370078740157477" bottom="0.39370078740157477" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" paperSize="8"/>
+  <pageSetup paperSize="8" orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>